<commit_message>
Update Energy Service Demands
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625CEEE-1548-49A0-A61C-BB752D361576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017E3134-A32B-4F51-85A5-99E9FE2E430F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="2235" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -13551,6 +13551,18 @@
     <xf numFmtId="0" fontId="62" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="27" borderId="1" xfId="14" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="26" borderId="1" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="26" borderId="47" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -13688,18 +13700,6 @@
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="27" borderId="1" xfId="14" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="26" borderId="1" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="26" borderId="47" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -14457,10 +14457,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14938,14 +14934,14 @@
       <c r="F16" s="156"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="518" t="s">
+      <c r="A17" s="522" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="518"/>
-      <c r="C17" s="518"/>
-      <c r="D17" s="518"/>
-      <c r="E17" s="518"/>
-      <c r="F17" s="518"/>
+      <c r="B17" s="522"/>
+      <c r="C17" s="522"/>
+      <c r="D17" s="522"/>
+      <c r="E17" s="522"/>
+      <c r="F17" s="522"/>
       <c r="G17" s="158"/>
       <c r="H17" s="158"/>
       <c r="I17" s="159"/>
@@ -14983,13 +14979,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="519" t="s">
+      <c r="B20" s="523" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="519"/>
-      <c r="D20" s="519"/>
-      <c r="E20" s="519"/>
-      <c r="F20" s="519"/>
+      <c r="C20" s="523"/>
+      <c r="D20" s="523"/>
+      <c r="E20" s="523"/>
+      <c r="F20" s="523"/>
       <c r="G20" s="163"/>
       <c r="H20" s="163"/>
       <c r="I20" s="164"/>
@@ -15003,13 +14999,13 @@
       <c r="A21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="520" t="s">
+      <c r="B21" s="524" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="520"/>
-      <c r="D21" s="520"/>
-      <c r="E21" s="520"/>
-      <c r="F21" s="520"/>
+      <c r="C21" s="524"/>
+      <c r="D21" s="524"/>
+      <c r="E21" s="524"/>
+      <c r="F21" s="524"/>
       <c r="G21" s="163"/>
       <c r="H21" s="163"/>
       <c r="I21" s="164"/>
@@ -15023,13 +15019,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="520" t="s">
+      <c r="B22" s="524" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="520"/>
-      <c r="D22" s="520"/>
-      <c r="E22" s="520"/>
-      <c r="F22" s="520"/>
+      <c r="C22" s="524"/>
+      <c r="D22" s="524"/>
+      <c r="E22" s="524"/>
+      <c r="F22" s="524"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -15058,22 +15054,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="521"/>
-      <c r="B25" s="521"/>
-      <c r="C25" s="521"/>
-      <c r="D25" s="521"/>
-      <c r="E25" s="521"/>
-      <c r="F25" s="521"/>
+      <c r="A25" s="525"/>
+      <c r="B25" s="525"/>
+      <c r="C25" s="525"/>
+      <c r="D25" s="525"/>
+      <c r="E25" s="525"/>
+      <c r="F25" s="525"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="517"/>
-      <c r="B26" s="517"/>
-      <c r="C26" s="517"/>
-      <c r="D26" s="517"/>
-      <c r="E26" s="517"/>
-      <c r="F26" s="517"/>
+      <c r="A26" s="521"/>
+      <c r="B26" s="521"/>
+      <c r="C26" s="521"/>
+      <c r="D26" s="521"/>
+      <c r="E26" s="521"/>
+      <c r="F26" s="521"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="156"/>
@@ -15260,16 +15256,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="522" t="s">
+      <c r="B2" s="526" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="523"/>
-      <c r="D2" s="523"/>
-      <c r="E2" s="524"/>
-      <c r="G2" s="522" t="s">
+      <c r="C2" s="527"/>
+      <c r="D2" s="527"/>
+      <c r="E2" s="528"/>
+      <c r="G2" s="526" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="524"/>
+      <c r="H2" s="528"/>
       <c r="I2" s="166"/>
       <c r="J2" s="166"/>
       <c r="K2" s="167"/>
@@ -15552,10 +15548,10 @@
       <c r="E14" s="182" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="522" t="s">
+      <c r="G14" s="526" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="524"/>
+      <c r="H14" s="528"/>
     </row>
     <row r="15" spans="2:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="179" t="s">
@@ -15639,12 +15635,12 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="525" t="s">
+      <c r="B20" s="529" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="526"/>
-      <c r="D20" s="526"/>
-      <c r="E20" s="527"/>
+      <c r="C20" s="530"/>
+      <c r="D20" s="530"/>
+      <c r="E20" s="531"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="194" t="s">
@@ -15827,16 +15823,16 @@
     </row>
     <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="522" t="s">
+      <c r="B36" s="526" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="523"/>
-      <c r="D36" s="523"/>
-      <c r="E36" s="524"/>
-      <c r="G36" s="528" t="s">
+      <c r="C36" s="527"/>
+      <c r="D36" s="527"/>
+      <c r="E36" s="528"/>
+      <c r="G36" s="532" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="529"/>
+      <c r="H36" s="533"/>
     </row>
     <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="210" t="s">
@@ -15934,7 +15930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4660B878-9B9C-4131-8EFF-29EF25ED69C5}">
   <dimension ref="A2:AL103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -15995,13 +15991,13 @@
       <c r="J3" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="530" t="s">
+      <c r="S3" s="534" t="s">
         <v>278</v>
       </c>
-      <c r="T3" s="530"/>
-      <c r="U3" s="530"/>
-      <c r="V3" s="530"/>
-      <c r="W3" s="530"/>
+      <c r="T3" s="534"/>
+      <c r="U3" s="534"/>
+      <c r="V3" s="534"/>
+      <c r="W3" s="534"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="19" t="s">
@@ -16055,10 +16051,10 @@
       <c r="J5" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="M5" s="563" t="s">
+      <c r="M5" s="517" t="s">
         <v>71</v>
       </c>
-      <c r="N5" s="563"/>
+      <c r="N5" s="517"/>
       <c r="S5" s="233" t="s">
         <v>263</v>
       </c>
@@ -16106,7 +16102,7 @@
       <c r="M6" s="233" t="s">
         <v>732</v>
       </c>
-      <c r="N6" s="566">
+      <c r="N6" s="520">
         <v>0.9</v>
       </c>
       <c r="S6" s="236" t="s">
@@ -16142,7 +16138,7 @@
       <c r="M7" s="236" t="s">
         <v>733</v>
       </c>
-      <c r="N7" s="564">
+      <c r="N7" s="518">
         <v>1</v>
       </c>
       <c r="S7" s="239" t="s">
@@ -16178,7 +16174,7 @@
       <c r="M8" s="239" t="s">
         <v>734</v>
       </c>
-      <c r="N8" s="565">
+      <c r="N8" s="519">
         <f>N6*0.7</f>
         <v>0.63</v>
       </c>
@@ -16215,7 +16211,7 @@
       <c r="M9" s="236" t="s">
         <v>735</v>
       </c>
-      <c r="N9" s="564">
+      <c r="N9" s="518">
         <v>0.4</v>
       </c>
       <c r="S9" s="239" t="s">
@@ -16251,7 +16247,7 @@
       <c r="M10" s="239" t="s">
         <v>736</v>
       </c>
-      <c r="N10" s="565">
+      <c r="N10" s="519">
         <v>0.6</v>
       </c>
       <c r="S10" s="236" t="s">
@@ -19021,34 +19017,34 @@
       <c r="G4" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="537" t="s">
+      <c r="H4" s="541" t="s">
         <v>304</v>
       </c>
-      <c r="I4" s="538"/>
-      <c r="J4" s="538"/>
-      <c r="K4" s="539"/>
-      <c r="L4" s="537" t="s">
+      <c r="I4" s="542"/>
+      <c r="J4" s="542"/>
+      <c r="K4" s="543"/>
+      <c r="L4" s="541" t="s">
         <v>89</v>
       </c>
-      <c r="M4" s="538"/>
-      <c r="N4" s="538"/>
-      <c r="O4" s="539"/>
-      <c r="P4" s="537" t="s">
+      <c r="M4" s="542"/>
+      <c r="N4" s="542"/>
+      <c r="O4" s="543"/>
+      <c r="P4" s="541" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="538"/>
-      <c r="R4" s="538"/>
-      <c r="S4" s="539"/>
-      <c r="T4" s="537" t="s">
+      <c r="Q4" s="542"/>
+      <c r="R4" s="542"/>
+      <c r="S4" s="543"/>
+      <c r="T4" s="541" t="s">
         <v>91</v>
       </c>
-      <c r="U4" s="539"/>
-      <c r="V4" s="531" t="s">
+      <c r="U4" s="543"/>
+      <c r="V4" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="W4" s="532"/>
-      <c r="X4" s="532"/>
-      <c r="Y4" s="533"/>
+      <c r="W4" s="536"/>
+      <c r="X4" s="536"/>
+      <c r="Y4" s="537"/>
       <c r="Z4" s="63"/>
       <c r="AA4" s="63"/>
       <c r="AB4" s="71" t="s">
@@ -19147,34 +19143,34 @@
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
       <c r="G6" s="42"/>
-      <c r="H6" s="534" t="s">
+      <c r="H6" s="538" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="535"/>
-      <c r="J6" s="535"/>
-      <c r="K6" s="536"/>
-      <c r="L6" s="535" t="s">
+      <c r="I6" s="539"/>
+      <c r="J6" s="539"/>
+      <c r="K6" s="540"/>
+      <c r="L6" s="539" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="535"/>
-      <c r="N6" s="535"/>
-      <c r="O6" s="536"/>
-      <c r="P6" s="534" t="s">
+      <c r="M6" s="539"/>
+      <c r="N6" s="539"/>
+      <c r="O6" s="540"/>
+      <c r="P6" s="538" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="535"/>
-      <c r="R6" s="535"/>
-      <c r="S6" s="536"/>
-      <c r="T6" s="534" t="s">
+      <c r="Q6" s="539"/>
+      <c r="R6" s="539"/>
+      <c r="S6" s="540"/>
+      <c r="T6" s="538" t="s">
         <v>74</v>
       </c>
-      <c r="U6" s="536"/>
-      <c r="V6" s="534" t="s">
+      <c r="U6" s="540"/>
+      <c r="V6" s="538" t="s">
         <v>552</v>
       </c>
-      <c r="W6" s="535"/>
-      <c r="X6" s="535"/>
-      <c r="Y6" s="536"/>
+      <c r="W6" s="539"/>
+      <c r="X6" s="539"/>
+      <c r="Y6" s="540"/>
       <c r="Z6" s="64" t="s">
         <v>564</v>
       </c>
@@ -22171,34 +22167,34 @@
       <c r="G42" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H42" s="537" t="s">
+      <c r="H42" s="541" t="s">
         <v>88</v>
       </c>
-      <c r="I42" s="538"/>
-      <c r="J42" s="538"/>
-      <c r="K42" s="539"/>
-      <c r="L42" s="537" t="s">
+      <c r="I42" s="542"/>
+      <c r="J42" s="542"/>
+      <c r="K42" s="543"/>
+      <c r="L42" s="541" t="s">
         <v>89</v>
       </c>
-      <c r="M42" s="538"/>
-      <c r="N42" s="538"/>
-      <c r="O42" s="539"/>
-      <c r="P42" s="537" t="s">
+      <c r="M42" s="542"/>
+      <c r="N42" s="542"/>
+      <c r="O42" s="543"/>
+      <c r="P42" s="541" t="s">
         <v>90</v>
       </c>
-      <c r="Q42" s="538"/>
-      <c r="R42" s="538"/>
-      <c r="S42" s="539"/>
-      <c r="T42" s="537" t="s">
+      <c r="Q42" s="542"/>
+      <c r="R42" s="542"/>
+      <c r="S42" s="543"/>
+      <c r="T42" s="541" t="s">
         <v>91</v>
       </c>
-      <c r="U42" s="539"/>
-      <c r="V42" s="531" t="s">
+      <c r="U42" s="543"/>
+      <c r="V42" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="W42" s="532"/>
-      <c r="X42" s="532"/>
-      <c r="Y42" s="533"/>
+      <c r="W42" s="536"/>
+      <c r="X42" s="536"/>
+      <c r="Y42" s="537"/>
       <c r="Z42" s="63"/>
       <c r="AA42" s="63"/>
       <c r="AB42" s="71" t="s">
@@ -22297,34 +22293,34 @@
       <c r="E44" s="41"/>
       <c r="F44" s="41"/>
       <c r="G44" s="42"/>
-      <c r="H44" s="534" t="s">
+      <c r="H44" s="538" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="535"/>
-      <c r="J44" s="535"/>
-      <c r="K44" s="536"/>
-      <c r="L44" s="535" t="s">
+      <c r="I44" s="539"/>
+      <c r="J44" s="539"/>
+      <c r="K44" s="540"/>
+      <c r="L44" s="539" t="s">
         <v>37</v>
       </c>
-      <c r="M44" s="535"/>
-      <c r="N44" s="535"/>
-      <c r="O44" s="536"/>
-      <c r="P44" s="534" t="s">
+      <c r="M44" s="539"/>
+      <c r="N44" s="539"/>
+      <c r="O44" s="540"/>
+      <c r="P44" s="538" t="s">
         <v>37</v>
       </c>
-      <c r="Q44" s="535"/>
-      <c r="R44" s="535"/>
-      <c r="S44" s="536"/>
-      <c r="T44" s="540" t="s">
+      <c r="Q44" s="539"/>
+      <c r="R44" s="539"/>
+      <c r="S44" s="540"/>
+      <c r="T44" s="544" t="s">
         <v>74</v>
       </c>
-      <c r="U44" s="541"/>
-      <c r="V44" s="540" t="s">
+      <c r="U44" s="545"/>
+      <c r="V44" s="544" t="s">
         <v>552</v>
       </c>
-      <c r="W44" s="542"/>
-      <c r="X44" s="542"/>
-      <c r="Y44" s="541"/>
+      <c r="W44" s="546"/>
+      <c r="X44" s="546"/>
+      <c r="Y44" s="545"/>
       <c r="Z44" s="389" t="s">
         <v>564</v>
       </c>
@@ -26081,34 +26077,34 @@
       <c r="G90" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H90" s="537" t="s">
+      <c r="H90" s="541" t="s">
         <v>88</v>
       </c>
-      <c r="I90" s="538"/>
-      <c r="J90" s="538"/>
-      <c r="K90" s="539"/>
-      <c r="L90" s="537" t="s">
+      <c r="I90" s="542"/>
+      <c r="J90" s="542"/>
+      <c r="K90" s="543"/>
+      <c r="L90" s="541" t="s">
         <v>89</v>
       </c>
-      <c r="M90" s="538"/>
-      <c r="N90" s="538"/>
-      <c r="O90" s="539"/>
-      <c r="P90" s="537" t="s">
+      <c r="M90" s="542"/>
+      <c r="N90" s="542"/>
+      <c r="O90" s="543"/>
+      <c r="P90" s="541" t="s">
         <v>90</v>
       </c>
-      <c r="Q90" s="538"/>
-      <c r="R90" s="538"/>
-      <c r="S90" s="539"/>
-      <c r="T90" s="537" t="s">
+      <c r="Q90" s="542"/>
+      <c r="R90" s="542"/>
+      <c r="S90" s="543"/>
+      <c r="T90" s="541" t="s">
         <v>91</v>
       </c>
-      <c r="U90" s="539"/>
-      <c r="V90" s="531" t="s">
+      <c r="U90" s="543"/>
+      <c r="V90" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="W90" s="532"/>
-      <c r="X90" s="532"/>
-      <c r="Y90" s="533"/>
+      <c r="W90" s="536"/>
+      <c r="X90" s="536"/>
+      <c r="Y90" s="537"/>
       <c r="Z90" s="63"/>
       <c r="AA90" s="63"/>
       <c r="AB90" s="71" t="s">
@@ -26207,34 +26203,34 @@
       <c r="E92" s="41"/>
       <c r="F92" s="41"/>
       <c r="G92" s="42"/>
-      <c r="H92" s="534" t="s">
+      <c r="H92" s="538" t="s">
         <v>37</v>
       </c>
-      <c r="I92" s="535"/>
-      <c r="J92" s="535"/>
-      <c r="K92" s="536"/>
-      <c r="L92" s="535" t="s">
+      <c r="I92" s="539"/>
+      <c r="J92" s="539"/>
+      <c r="K92" s="540"/>
+      <c r="L92" s="539" t="s">
         <v>37</v>
       </c>
-      <c r="M92" s="535"/>
-      <c r="N92" s="535"/>
-      <c r="O92" s="536"/>
-      <c r="P92" s="534" t="s">
+      <c r="M92" s="539"/>
+      <c r="N92" s="539"/>
+      <c r="O92" s="540"/>
+      <c r="P92" s="538" t="s">
         <v>37</v>
       </c>
-      <c r="Q92" s="535"/>
-      <c r="R92" s="535"/>
-      <c r="S92" s="536"/>
-      <c r="T92" s="540" t="s">
+      <c r="Q92" s="539"/>
+      <c r="R92" s="539"/>
+      <c r="S92" s="540"/>
+      <c r="T92" s="544" t="s">
         <v>74</v>
       </c>
-      <c r="U92" s="541"/>
-      <c r="V92" s="540" t="s">
+      <c r="U92" s="545"/>
+      <c r="V92" s="544" t="s">
         <v>552</v>
       </c>
-      <c r="W92" s="542"/>
-      <c r="X92" s="542"/>
-      <c r="Y92" s="541"/>
+      <c r="W92" s="546"/>
+      <c r="X92" s="546"/>
+      <c r="Y92" s="545"/>
       <c r="Z92" s="389" t="s">
         <v>564</v>
       </c>
@@ -30327,12 +30323,12 @@
       <c r="I5" s="130"/>
       <c r="J5" s="130"/>
       <c r="K5" s="130"/>
-      <c r="L5" s="531" t="s">
+      <c r="L5" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="M5" s="532"/>
-      <c r="N5" s="532"/>
-      <c r="O5" s="533"/>
+      <c r="M5" s="536"/>
+      <c r="N5" s="536"/>
+      <c r="O5" s="537"/>
       <c r="P5" s="63"/>
       <c r="Q5" s="63" t="s">
         <v>93</v>
@@ -30363,12 +30359,12 @@
       <c r="I6" s="40"/>
       <c r="J6" s="40"/>
       <c r="K6" s="40"/>
-      <c r="L6" s="540" t="s">
+      <c r="L6" s="544" t="s">
         <v>552</v>
       </c>
-      <c r="M6" s="542"/>
-      <c r="N6" s="542"/>
-      <c r="O6" s="541"/>
+      <c r="M6" s="546"/>
+      <c r="N6" s="546"/>
+      <c r="O6" s="545"/>
       <c r="P6" s="389" t="s">
         <v>564</v>
       </c>
@@ -31254,23 +31250,23 @@
       <c r="K33" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L33" s="531" t="s">
+      <c r="L33" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="M33" s="532"/>
-      <c r="N33" s="532"/>
-      <c r="O33" s="533"/>
+      <c r="M33" s="536"/>
+      <c r="N33" s="536"/>
+      <c r="O33" s="537"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="L34" s="540" t="s">
+      <c r="L34" s="544" t="s">
         <v>97</v>
       </c>
-      <c r="M34" s="542"/>
-      <c r="N34" s="542"/>
-      <c r="O34" s="541"/>
+      <c r="M34" s="546"/>
+      <c r="N34" s="546"/>
+      <c r="O34" s="545"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -31611,16 +31607,16 @@
       <c r="G4" s="130" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="537" t="s">
+      <c r="H4" s="541" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="538"/>
-      <c r="J4" s="539"/>
-      <c r="K4" s="531" t="s">
+      <c r="I4" s="542"/>
+      <c r="J4" s="543"/>
+      <c r="K4" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="532"/>
-      <c r="M4" s="533"/>
+      <c r="L4" s="536"/>
+      <c r="M4" s="537"/>
       <c r="N4" s="63"/>
       <c r="O4" s="63" t="s">
         <v>93</v>
@@ -31646,16 +31642,16 @@
       <c r="G5" s="397" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="543" t="s">
+      <c r="H5" s="547" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="544"/>
-      <c r="J5" s="545"/>
-      <c r="K5" s="543" t="s">
+      <c r="I5" s="548"/>
+      <c r="J5" s="549"/>
+      <c r="K5" s="547" t="s">
         <v>341</v>
       </c>
-      <c r="L5" s="544"/>
-      <c r="M5" s="545"/>
+      <c r="L5" s="548"/>
+      <c r="M5" s="549"/>
       <c r="N5" s="398" t="s">
         <v>98</v>
       </c>
@@ -31672,23 +31668,23 @@
         <v>226</v>
       </c>
       <c r="AA5" s="220"/>
-      <c r="AB5" s="546" t="s">
+      <c r="AB5" s="550" t="s">
         <v>594</v>
       </c>
-      <c r="AC5" s="546"/>
+      <c r="AC5" s="550"/>
       <c r="AD5" s="400"/>
-      <c r="AE5" s="547" t="s">
+      <c r="AE5" s="551" t="s">
         <v>71</v>
       </c>
-      <c r="AF5" s="547"/>
-      <c r="AG5" s="547" t="s">
+      <c r="AF5" s="551"/>
+      <c r="AG5" s="551" t="s">
         <v>595</v>
       </c>
-      <c r="AH5" s="547"/>
-      <c r="AI5" s="548" t="s">
+      <c r="AH5" s="551"/>
+      <c r="AI5" s="552" t="s">
         <v>596</v>
       </c>
-      <c r="AJ5" s="548"/>
+      <c r="AJ5" s="552"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="444" t="str">
@@ -32426,12 +32422,12 @@
       <c r="K27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L27" s="531" t="s">
+      <c r="L27" s="535" t="s">
         <v>92</v>
       </c>
-      <c r="M27" s="532"/>
-      <c r="N27" s="532"/>
-      <c r="O27" s="533"/>
+      <c r="M27" s="536"/>
+      <c r="N27" s="536"/>
+      <c r="O27" s="537"/>
       <c r="T27" s="222"/>
       <c r="U27" s="222"/>
     </row>
@@ -32439,12 +32435,12 @@
       <c r="J28" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="L28" s="534" t="s">
+      <c r="L28" s="538" t="s">
         <v>97</v>
       </c>
-      <c r="M28" s="535"/>
-      <c r="N28" s="535"/>
-      <c r="O28" s="536"/>
+      <c r="M28" s="539"/>
+      <c r="N28" s="539"/>
+      <c r="O28" s="540"/>
       <c r="T28" s="222"/>
       <c r="U28" s="222"/>
     </row>
@@ -34273,128 +34269,128 @@
       <c r="C4" s="295" t="s">
         <v>350</v>
       </c>
-      <c r="D4" s="549" t="s">
+      <c r="D4" s="553" t="s">
         <v>351</v>
       </c>
-      <c r="E4" s="550"/>
-      <c r="F4" s="550"/>
-      <c r="G4" s="550"/>
-      <c r="H4" s="551"/>
-      <c r="I4" s="550" t="s">
+      <c r="E4" s="554"/>
+      <c r="F4" s="554"/>
+      <c r="G4" s="554"/>
+      <c r="H4" s="555"/>
+      <c r="I4" s="554" t="s">
         <v>352</v>
       </c>
-      <c r="J4" s="550"/>
-      <c r="K4" s="550"/>
-      <c r="L4" s="550"/>
-      <c r="M4" s="551"/>
-      <c r="N4" s="550" t="s">
+      <c r="J4" s="554"/>
+      <c r="K4" s="554"/>
+      <c r="L4" s="554"/>
+      <c r="M4" s="555"/>
+      <c r="N4" s="554" t="s">
         <v>353</v>
       </c>
-      <c r="O4" s="550"/>
-      <c r="P4" s="550"/>
-      <c r="Q4" s="550"/>
-      <c r="R4" s="551"/>
-      <c r="S4" s="550" t="s">
+      <c r="O4" s="554"/>
+      <c r="P4" s="554"/>
+      <c r="Q4" s="554"/>
+      <c r="R4" s="555"/>
+      <c r="S4" s="554" t="s">
         <v>354</v>
       </c>
-      <c r="T4" s="550"/>
-      <c r="U4" s="550"/>
-      <c r="V4" s="550"/>
-      <c r="W4" s="551"/>
-      <c r="X4" s="550" t="s">
+      <c r="T4" s="554"/>
+      <c r="U4" s="554"/>
+      <c r="V4" s="554"/>
+      <c r="W4" s="555"/>
+      <c r="X4" s="554" t="s">
         <v>355</v>
       </c>
-      <c r="Y4" s="550"/>
-      <c r="Z4" s="550"/>
-      <c r="AA4" s="550"/>
-      <c r="AB4" s="551"/>
-      <c r="AC4" s="550" t="s">
+      <c r="Y4" s="554"/>
+      <c r="Z4" s="554"/>
+      <c r="AA4" s="554"/>
+      <c r="AB4" s="555"/>
+      <c r="AC4" s="554" t="s">
         <v>356</v>
       </c>
-      <c r="AD4" s="550"/>
-      <c r="AE4" s="550"/>
-      <c r="AF4" s="550"/>
-      <c r="AG4" s="551"/>
-      <c r="AH4" s="550" t="s">
+      <c r="AD4" s="554"/>
+      <c r="AE4" s="554"/>
+      <c r="AF4" s="554"/>
+      <c r="AG4" s="555"/>
+      <c r="AH4" s="554" t="s">
         <v>357</v>
       </c>
-      <c r="AI4" s="550"/>
-      <c r="AJ4" s="550"/>
-      <c r="AK4" s="550"/>
-      <c r="AL4" s="551"/>
-      <c r="AM4" s="550" t="s">
+      <c r="AI4" s="554"/>
+      <c r="AJ4" s="554"/>
+      <c r="AK4" s="554"/>
+      <c r="AL4" s="555"/>
+      <c r="AM4" s="554" t="s">
         <v>358</v>
       </c>
-      <c r="AN4" s="550"/>
-      <c r="AO4" s="550"/>
-      <c r="AP4" s="550"/>
-      <c r="AQ4" s="551"/>
-      <c r="AR4" s="550" t="s">
+      <c r="AN4" s="554"/>
+      <c r="AO4" s="554"/>
+      <c r="AP4" s="554"/>
+      <c r="AQ4" s="555"/>
+      <c r="AR4" s="554" t="s">
         <v>359</v>
       </c>
-      <c r="AS4" s="550"/>
-      <c r="AT4" s="550"/>
-      <c r="AU4" s="550"/>
-      <c r="AV4" s="551"/>
-      <c r="AW4" s="550" t="s">
+      <c r="AS4" s="554"/>
+      <c r="AT4" s="554"/>
+      <c r="AU4" s="554"/>
+      <c r="AV4" s="555"/>
+      <c r="AW4" s="554" t="s">
         <v>360</v>
       </c>
-      <c r="AX4" s="550"/>
-      <c r="AY4" s="550"/>
-      <c r="AZ4" s="550"/>
-      <c r="BA4" s="550"/>
-      <c r="BB4" s="549" t="s">
+      <c r="AX4" s="554"/>
+      <c r="AY4" s="554"/>
+      <c r="AZ4" s="554"/>
+      <c r="BA4" s="554"/>
+      <c r="BB4" s="553" t="s">
         <v>361</v>
       </c>
-      <c r="BC4" s="550"/>
-      <c r="BD4" s="550"/>
-      <c r="BE4" s="550"/>
-      <c r="BF4" s="551"/>
-      <c r="BG4" s="550" t="s">
+      <c r="BC4" s="554"/>
+      <c r="BD4" s="554"/>
+      <c r="BE4" s="554"/>
+      <c r="BF4" s="555"/>
+      <c r="BG4" s="554" t="s">
         <v>362</v>
       </c>
-      <c r="BH4" s="550"/>
-      <c r="BI4" s="550"/>
-      <c r="BJ4" s="550"/>
-      <c r="BK4" s="550"/>
-      <c r="BL4" s="549" t="s">
+      <c r="BH4" s="554"/>
+      <c r="BI4" s="554"/>
+      <c r="BJ4" s="554"/>
+      <c r="BK4" s="554"/>
+      <c r="BL4" s="553" t="s">
         <v>363</v>
       </c>
-      <c r="BM4" s="550"/>
-      <c r="BN4" s="550"/>
-      <c r="BO4" s="550"/>
-      <c r="BP4" s="550"/>
-      <c r="BQ4" s="549" t="s">
+      <c r="BM4" s="554"/>
+      <c r="BN4" s="554"/>
+      <c r="BO4" s="554"/>
+      <c r="BP4" s="554"/>
+      <c r="BQ4" s="553" t="s">
         <v>364</v>
       </c>
-      <c r="BR4" s="550"/>
-      <c r="BS4" s="550"/>
-      <c r="BT4" s="550"/>
-      <c r="BU4" s="551"/>
+      <c r="BR4" s="554"/>
+      <c r="BS4" s="554"/>
+      <c r="BT4" s="554"/>
+      <c r="BU4" s="555"/>
       <c r="BV4" s="296" t="s">
         <v>365</v>
       </c>
-      <c r="BW4" s="552" t="s">
+      <c r="BW4" s="556" t="s">
         <v>366</v>
       </c>
-      <c r="BX4" s="553"/>
-      <c r="BY4" s="553"/>
-      <c r="BZ4" s="553"/>
-      <c r="CA4" s="554"/>
-      <c r="CB4" s="552" t="s">
+      <c r="BX4" s="557"/>
+      <c r="BY4" s="557"/>
+      <c r="BZ4" s="557"/>
+      <c r="CA4" s="558"/>
+      <c r="CB4" s="556" t="s">
         <v>367</v>
       </c>
-      <c r="CC4" s="553"/>
-      <c r="CD4" s="553"/>
-      <c r="CE4" s="553"/>
-      <c r="CF4" s="554"/>
-      <c r="CG4" s="552" t="s">
+      <c r="CC4" s="557"/>
+      <c r="CD4" s="557"/>
+      <c r="CE4" s="557"/>
+      <c r="CF4" s="558"/>
+      <c r="CG4" s="556" t="s">
         <v>368</v>
       </c>
-      <c r="CH4" s="553"/>
-      <c r="CI4" s="553"/>
-      <c r="CJ4" s="553"/>
-      <c r="CK4" s="554"/>
+      <c r="CH4" s="557"/>
+      <c r="CI4" s="557"/>
+      <c r="CJ4" s="557"/>
+      <c r="CK4" s="558"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="298"/>
@@ -48001,23 +47997,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="556" t="s">
+      <c r="A1" s="560" t="s">
         <v>638</v>
       </c>
-      <c r="B1" s="558" t="s">
+      <c r="B1" s="562" t="s">
         <v>639</v>
       </c>
-      <c r="C1" s="559"/>
-      <c r="D1" s="559"/>
-      <c r="E1" s="559"/>
-      <c r="F1" s="560"/>
-      <c r="G1" s="558" t="s">
+      <c r="C1" s="563"/>
+      <c r="D1" s="563"/>
+      <c r="E1" s="563"/>
+      <c r="F1" s="564"/>
+      <c r="G1" s="562" t="s">
         <v>640</v>
       </c>
-      <c r="H1" s="559"/>
-      <c r="I1" s="559"/>
-      <c r="J1" s="559"/>
-      <c r="K1" s="560"/>
+      <c r="H1" s="563"/>
+      <c r="I1" s="563"/>
+      <c r="J1" s="563"/>
+      <c r="K1" s="564"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -48027,7 +48023,7 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="557"/>
+      <c r="A2" s="561"/>
       <c r="B2" s="466" t="s">
         <v>284</v>
       </c>
@@ -48173,12 +48169,12 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="555" t="s">
+      <c r="A7" s="559" t="s">
         <v>641</v>
       </c>
-      <c r="B7" s="555"/>
-      <c r="C7" s="555"/>
-      <c r="D7" s="555"/>
+      <c r="B7" s="559"/>
+      <c r="C7" s="559"/>
+      <c r="D7" s="559"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -48464,12 +48460,12 @@
       <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="555" t="s">
+      <c r="A18" s="559" t="s">
         <v>655</v>
       </c>
-      <c r="B18" s="555"/>
-      <c r="C18" s="555"/>
-      <c r="D18" s="555"/>
+      <c r="B18" s="559"/>
+      <c r="C18" s="559"/>
+      <c r="D18" s="559"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -48724,12 +48720,12 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="555" t="s">
+      <c r="A28" s="559" t="s">
         <v>663</v>
       </c>
-      <c r="B28" s="555"/>
-      <c r="C28" s="555"/>
-      <c r="D28" s="555"/>
+      <c r="B28" s="559"/>
+      <c r="C28" s="559"/>
+      <c r="D28" s="559"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -49217,12 +49213,12 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="555" t="s">
+      <c r="A40" s="559" t="s">
         <v>644</v>
       </c>
-      <c r="B40" s="555"/>
-      <c r="C40" s="555"/>
-      <c r="D40" s="555"/>
+      <c r="B40" s="559"/>
+      <c r="C40" s="559"/>
+      <c r="D40" s="559"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -49398,12 +49394,12 @@
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="555" t="s">
+      <c r="A45" s="559" t="s">
         <v>672</v>
       </c>
-      <c r="B45" s="555"/>
-      <c r="C45" s="555"/>
-      <c r="D45" s="555"/>
+      <c r="B45" s="559"/>
+      <c r="C45" s="559"/>
+      <c r="D45" s="559"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -49520,11 +49516,11 @@
       <c r="Y48" t="s">
         <v>689</v>
       </c>
-      <c r="Z48" s="561" t="s">
+      <c r="Z48" s="565" t="s">
         <v>627</v>
       </c>
-      <c r="AA48" s="562"/>
-      <c r="AB48" s="562"/>
+      <c r="AA48" s="566"/>
+      <c r="AB48" s="566"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -49741,11 +49737,11 @@
       <c r="Y53" t="s">
         <v>691</v>
       </c>
-      <c r="Z53" s="561" t="s">
+      <c r="Z53" s="565" t="s">
         <v>626</v>
       </c>
-      <c r="AA53" s="562"/>
-      <c r="AB53" s="562"/>
+      <c r="AA53" s="566"/>
+      <c r="AB53" s="566"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -49947,11 +49943,11 @@
       <c r="Y59" t="s">
         <v>692</v>
       </c>
-      <c r="Z59" s="561" t="s">
+      <c r="Z59" s="565" t="s">
         <v>693</v>
       </c>
-      <c r="AA59" s="562"/>
-      <c r="AB59" s="562"/>
+      <c r="AA59" s="566"/>
+      <c r="AB59" s="566"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="486" t="str">

</xml_diff>

<commit_message>
Return electric heater price - still issues with no retrofits.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC20BE32-78B0-4D3D-8D7F-14F41295A8B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA717D5-1D02-42A5-831C-4F0884BDFE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -13605,15 +13605,6 @@
     <xf numFmtId="0" fontId="42" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13621,6 +13612,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13632,22 +13632,13 @@
     <xf numFmtId="0" fontId="17" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -13659,10 +13650,19 @@
     <xf numFmtId="0" fontId="58" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="29" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="29" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13680,6 +13680,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13694,12 +13700,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -18852,8 +18852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AR166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E27" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X68" sqref="X68"/>
+    <sheetView tabSelected="1" topLeftCell="E69" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X114" sqref="X114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19039,12 +19039,12 @@
         <v>91</v>
       </c>
       <c r="U4" s="543"/>
-      <c r="V4" s="535" t="s">
+      <c r="V4" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="W4" s="536"/>
-      <c r="X4" s="536"/>
-      <c r="Y4" s="537"/>
+      <c r="W4" s="545"/>
+      <c r="X4" s="545"/>
+      <c r="Y4" s="546"/>
       <c r="Z4" s="63"/>
       <c r="AA4" s="63"/>
       <c r="AB4" s="71" t="s">
@@ -19143,34 +19143,34 @@
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
       <c r="G6" s="42"/>
-      <c r="H6" s="538" t="s">
+      <c r="H6" s="535" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="539"/>
-      <c r="J6" s="539"/>
-      <c r="K6" s="540"/>
-      <c r="L6" s="539" t="s">
+      <c r="I6" s="536"/>
+      <c r="J6" s="536"/>
+      <c r="K6" s="537"/>
+      <c r="L6" s="536" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="539"/>
-      <c r="N6" s="539"/>
-      <c r="O6" s="540"/>
-      <c r="P6" s="538" t="s">
+      <c r="M6" s="536"/>
+      <c r="N6" s="536"/>
+      <c r="O6" s="537"/>
+      <c r="P6" s="535" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="539"/>
-      <c r="R6" s="539"/>
-      <c r="S6" s="540"/>
-      <c r="T6" s="538" t="s">
+      <c r="Q6" s="536"/>
+      <c r="R6" s="536"/>
+      <c r="S6" s="537"/>
+      <c r="T6" s="535" t="s">
         <v>74</v>
       </c>
-      <c r="U6" s="540"/>
-      <c r="V6" s="538" t="s">
+      <c r="U6" s="537"/>
+      <c r="V6" s="535" t="s">
         <v>552</v>
       </c>
-      <c r="W6" s="539"/>
-      <c r="X6" s="539"/>
-      <c r="Y6" s="540"/>
+      <c r="W6" s="536"/>
+      <c r="X6" s="536"/>
+      <c r="Y6" s="537"/>
       <c r="Z6" s="64" t="s">
         <v>564</v>
       </c>
@@ -22189,12 +22189,12 @@
         <v>91</v>
       </c>
       <c r="U42" s="543"/>
-      <c r="V42" s="535" t="s">
+      <c r="V42" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="W42" s="536"/>
-      <c r="X42" s="536"/>
-      <c r="Y42" s="537"/>
+      <c r="W42" s="545"/>
+      <c r="X42" s="545"/>
+      <c r="Y42" s="546"/>
       <c r="Z42" s="63"/>
       <c r="AA42" s="63"/>
       <c r="AB42" s="71" t="s">
@@ -22293,34 +22293,34 @@
       <c r="E44" s="41"/>
       <c r="F44" s="41"/>
       <c r="G44" s="42"/>
-      <c r="H44" s="538" t="s">
+      <c r="H44" s="535" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="539"/>
-      <c r="J44" s="539"/>
-      <c r="K44" s="540"/>
-      <c r="L44" s="539" t="s">
+      <c r="I44" s="536"/>
+      <c r="J44" s="536"/>
+      <c r="K44" s="537"/>
+      <c r="L44" s="536" t="s">
         <v>37</v>
       </c>
-      <c r="M44" s="539"/>
-      <c r="N44" s="539"/>
-      <c r="O44" s="540"/>
-      <c r="P44" s="538" t="s">
+      <c r="M44" s="536"/>
+      <c r="N44" s="536"/>
+      <c r="O44" s="537"/>
+      <c r="P44" s="535" t="s">
         <v>37</v>
       </c>
-      <c r="Q44" s="539"/>
-      <c r="R44" s="539"/>
-      <c r="S44" s="540"/>
-      <c r="T44" s="544" t="s">
+      <c r="Q44" s="536"/>
+      <c r="R44" s="536"/>
+      <c r="S44" s="537"/>
+      <c r="T44" s="538" t="s">
         <v>74</v>
       </c>
-      <c r="U44" s="545"/>
-      <c r="V44" s="544" t="s">
+      <c r="U44" s="539"/>
+      <c r="V44" s="538" t="s">
         <v>552</v>
       </c>
-      <c r="W44" s="546"/>
-      <c r="X44" s="546"/>
-      <c r="Y44" s="545"/>
+      <c r="W44" s="540"/>
+      <c r="X44" s="540"/>
+      <c r="Y44" s="539"/>
       <c r="Z44" s="389" t="s">
         <v>564</v>
       </c>
@@ -24104,20 +24104,20 @@
       </c>
       <c r="U62" s="81"/>
       <c r="V62" s="82">
-        <f>(JRC_Data!BB48/1000)*($U$153/$U$151)</f>
-        <v>4.2809917355371896</v>
+        <f>(JRC_Data!BB48/1000)*($U$152/$U$151)</f>
+        <v>4.0495867768595044</v>
       </c>
       <c r="W62" s="82">
-        <f>(JRC_Data!BC48/1000)*($U$153/$U$151)</f>
-        <v>4.2809917355371896</v>
+        <f>(JRC_Data!BC48/1000)*($U$152/$U$151)</f>
+        <v>4.0495867768595044</v>
       </c>
       <c r="X62" s="82">
-        <f>(JRC_Data!BD48/1000)*($U$153/$U$151)</f>
-        <v>4.2809917355371896</v>
+        <f>(JRC_Data!BD48/1000)*($U$152/$U$151)</f>
+        <v>4.0495867768595044</v>
       </c>
       <c r="Y62" s="82">
-        <f>(JRC_Data!BE48/1000)*($U$153/$U$151)</f>
-        <v>4.2809917355371896</v>
+        <f>(JRC_Data!BE48/1000)*($U$152/$U$151)</f>
+        <v>4.0495867768595044</v>
       </c>
       <c r="Z62" s="85">
         <f>JRC_Data!BL48/1000</f>
@@ -26099,12 +26099,12 @@
         <v>91</v>
       </c>
       <c r="U90" s="543"/>
-      <c r="V90" s="535" t="s">
+      <c r="V90" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="W90" s="536"/>
-      <c r="X90" s="536"/>
-      <c r="Y90" s="537"/>
+      <c r="W90" s="545"/>
+      <c r="X90" s="545"/>
+      <c r="Y90" s="546"/>
       <c r="Z90" s="63"/>
       <c r="AA90" s="63"/>
       <c r="AB90" s="71" t="s">
@@ -26203,34 +26203,34 @@
       <c r="E92" s="41"/>
       <c r="F92" s="41"/>
       <c r="G92" s="42"/>
-      <c r="H92" s="538" t="s">
+      <c r="H92" s="535" t="s">
         <v>37</v>
       </c>
-      <c r="I92" s="539"/>
-      <c r="J92" s="539"/>
-      <c r="K92" s="540"/>
-      <c r="L92" s="539" t="s">
+      <c r="I92" s="536"/>
+      <c r="J92" s="536"/>
+      <c r="K92" s="537"/>
+      <c r="L92" s="536" t="s">
         <v>37</v>
       </c>
-      <c r="M92" s="539"/>
-      <c r="N92" s="539"/>
-      <c r="O92" s="540"/>
-      <c r="P92" s="538" t="s">
+      <c r="M92" s="536"/>
+      <c r="N92" s="536"/>
+      <c r="O92" s="537"/>
+      <c r="P92" s="535" t="s">
         <v>37</v>
       </c>
-      <c r="Q92" s="539"/>
-      <c r="R92" s="539"/>
-      <c r="S92" s="540"/>
-      <c r="T92" s="544" t="s">
+      <c r="Q92" s="536"/>
+      <c r="R92" s="536"/>
+      <c r="S92" s="537"/>
+      <c r="T92" s="538" t="s">
         <v>74</v>
       </c>
-      <c r="U92" s="545"/>
-      <c r="V92" s="544" t="s">
+      <c r="U92" s="539"/>
+      <c r="V92" s="538" t="s">
         <v>552</v>
       </c>
-      <c r="W92" s="546"/>
-      <c r="X92" s="546"/>
-      <c r="Y92" s="545"/>
+      <c r="W92" s="540"/>
+      <c r="X92" s="540"/>
+      <c r="Y92" s="539"/>
       <c r="Z92" s="389" t="s">
         <v>564</v>
       </c>
@@ -28014,20 +28014,20 @@
       </c>
       <c r="U110" s="81"/>
       <c r="V110" s="82">
-        <f>(JRC_Data!BB48/1000)*($U$154/$U$151)</f>
-        <v>4.6198347107438016</v>
+        <f>(JRC_Data!BB48/1000)*($U$153/$U$151)</f>
+        <v>4.2809917355371896</v>
       </c>
       <c r="W110" s="82">
-        <f>(JRC_Data!BC48/1000)*($U$154/$U$151)</f>
-        <v>4.6198347107438016</v>
+        <f>(JRC_Data!BC48/1000)*($U$153/$U$151)</f>
+        <v>4.2809917355371896</v>
       </c>
       <c r="X110" s="82">
-        <f>(JRC_Data!BD48/1000)*($U$154/$U$151)</f>
-        <v>4.6198347107438016</v>
+        <f>(JRC_Data!BD48/1000)*($U$153/$U$151)</f>
+        <v>4.2809917355371896</v>
       </c>
       <c r="Y110" s="82">
-        <f>(JRC_Data!BE48/1000)*($U$154/$U$151)</f>
-        <v>4.6198347107438016</v>
+        <f>(JRC_Data!BE48/1000)*($U$153/$U$151)</f>
+        <v>4.2809917355371896</v>
       </c>
       <c r="Z110" s="85">
         <f>JRC_Data!BL48/1000</f>
@@ -30149,26 +30149,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -30179,6 +30159,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -30323,12 +30323,12 @@
       <c r="I5" s="130"/>
       <c r="J5" s="130"/>
       <c r="K5" s="130"/>
-      <c r="L5" s="535" t="s">
+      <c r="L5" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="M5" s="536"/>
-      <c r="N5" s="536"/>
-      <c r="O5" s="537"/>
+      <c r="M5" s="545"/>
+      <c r="N5" s="545"/>
+      <c r="O5" s="546"/>
       <c r="P5" s="63"/>
       <c r="Q5" s="63" t="s">
         <v>93</v>
@@ -30359,12 +30359,12 @@
       <c r="I6" s="40"/>
       <c r="J6" s="40"/>
       <c r="K6" s="40"/>
-      <c r="L6" s="544" t="s">
+      <c r="L6" s="538" t="s">
         <v>552</v>
       </c>
-      <c r="M6" s="546"/>
-      <c r="N6" s="546"/>
-      <c r="O6" s="545"/>
+      <c r="M6" s="540"/>
+      <c r="N6" s="540"/>
+      <c r="O6" s="539"/>
       <c r="P6" s="389" t="s">
         <v>564</v>
       </c>
@@ -31250,23 +31250,23 @@
       <c r="K33" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L33" s="535" t="s">
+      <c r="L33" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="M33" s="536"/>
-      <c r="N33" s="536"/>
-      <c r="O33" s="537"/>
+      <c r="M33" s="545"/>
+      <c r="N33" s="545"/>
+      <c r="O33" s="546"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="L34" s="544" t="s">
+      <c r="L34" s="538" t="s">
         <v>97</v>
       </c>
-      <c r="M34" s="546"/>
-      <c r="N34" s="546"/>
-      <c r="O34" s="545"/>
+      <c r="M34" s="540"/>
+      <c r="N34" s="540"/>
+      <c r="O34" s="539"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -31612,11 +31612,11 @@
       </c>
       <c r="I4" s="542"/>
       <c r="J4" s="543"/>
-      <c r="K4" s="535" t="s">
+      <c r="K4" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="536"/>
-      <c r="M4" s="537"/>
+      <c r="L4" s="545"/>
+      <c r="M4" s="546"/>
       <c r="N4" s="63"/>
       <c r="O4" s="63" t="s">
         <v>93</v>
@@ -31642,16 +31642,16 @@
       <c r="G5" s="397" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="547" t="s">
+      <c r="H5" s="550" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="548"/>
-      <c r="J5" s="549"/>
-      <c r="K5" s="547" t="s">
+      <c r="I5" s="551"/>
+      <c r="J5" s="552"/>
+      <c r="K5" s="550" t="s">
         <v>341</v>
       </c>
-      <c r="L5" s="548"/>
-      <c r="M5" s="549"/>
+      <c r="L5" s="551"/>
+      <c r="M5" s="552"/>
       <c r="N5" s="398" t="s">
         <v>98</v>
       </c>
@@ -31668,23 +31668,23 @@
         <v>226</v>
       </c>
       <c r="AA5" s="220"/>
-      <c r="AB5" s="550" t="s">
+      <c r="AB5" s="547" t="s">
         <v>594</v>
       </c>
-      <c r="AC5" s="550"/>
+      <c r="AC5" s="547"/>
       <c r="AD5" s="400"/>
-      <c r="AE5" s="551" t="s">
+      <c r="AE5" s="548" t="s">
         <v>71</v>
       </c>
-      <c r="AF5" s="551"/>
-      <c r="AG5" s="551" t="s">
+      <c r="AF5" s="548"/>
+      <c r="AG5" s="548" t="s">
         <v>595</v>
       </c>
-      <c r="AH5" s="551"/>
-      <c r="AI5" s="552" t="s">
+      <c r="AH5" s="548"/>
+      <c r="AI5" s="549" t="s">
         <v>596</v>
       </c>
-      <c r="AJ5" s="552"/>
+      <c r="AJ5" s="549"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="444" t="str">
@@ -32422,12 +32422,12 @@
       <c r="K27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L27" s="535" t="s">
+      <c r="L27" s="544" t="s">
         <v>92</v>
       </c>
-      <c r="M27" s="536"/>
-      <c r="N27" s="536"/>
-      <c r="O27" s="537"/>
+      <c r="M27" s="545"/>
+      <c r="N27" s="545"/>
+      <c r="O27" s="546"/>
       <c r="T27" s="222"/>
       <c r="U27" s="222"/>
     </row>
@@ -32435,12 +32435,12 @@
       <c r="J28" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="L28" s="538" t="s">
+      <c r="L28" s="535" t="s">
         <v>97</v>
       </c>
-      <c r="M28" s="539"/>
-      <c r="N28" s="539"/>
-      <c r="O28" s="540"/>
+      <c r="M28" s="536"/>
+      <c r="N28" s="536"/>
+      <c r="O28" s="537"/>
       <c r="T28" s="222"/>
       <c r="U28" s="222"/>
     </row>
@@ -33830,16 +33830,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -34269,103 +34269,103 @@
       <c r="C4" s="295" t="s">
         <v>350</v>
       </c>
-      <c r="D4" s="553" t="s">
+      <c r="D4" s="554" t="s">
         <v>351</v>
       </c>
-      <c r="E4" s="554"/>
-      <c r="F4" s="554"/>
-      <c r="G4" s="554"/>
+      <c r="E4" s="553"/>
+      <c r="F4" s="553"/>
+      <c r="G4" s="553"/>
       <c r="H4" s="555"/>
-      <c r="I4" s="554" t="s">
+      <c r="I4" s="553" t="s">
         <v>352</v>
       </c>
-      <c r="J4" s="554"/>
-      <c r="K4" s="554"/>
-      <c r="L4" s="554"/>
+      <c r="J4" s="553"/>
+      <c r="K4" s="553"/>
+      <c r="L4" s="553"/>
       <c r="M4" s="555"/>
-      <c r="N4" s="554" t="s">
+      <c r="N4" s="553" t="s">
         <v>353</v>
       </c>
-      <c r="O4" s="554"/>
-      <c r="P4" s="554"/>
-      <c r="Q4" s="554"/>
+      <c r="O4" s="553"/>
+      <c r="P4" s="553"/>
+      <c r="Q4" s="553"/>
       <c r="R4" s="555"/>
-      <c r="S4" s="554" t="s">
+      <c r="S4" s="553" t="s">
         <v>354</v>
       </c>
-      <c r="T4" s="554"/>
-      <c r="U4" s="554"/>
-      <c r="V4" s="554"/>
+      <c r="T4" s="553"/>
+      <c r="U4" s="553"/>
+      <c r="V4" s="553"/>
       <c r="W4" s="555"/>
-      <c r="X4" s="554" t="s">
+      <c r="X4" s="553" t="s">
         <v>355</v>
       </c>
-      <c r="Y4" s="554"/>
-      <c r="Z4" s="554"/>
-      <c r="AA4" s="554"/>
+      <c r="Y4" s="553"/>
+      <c r="Z4" s="553"/>
+      <c r="AA4" s="553"/>
       <c r="AB4" s="555"/>
-      <c r="AC4" s="554" t="s">
+      <c r="AC4" s="553" t="s">
         <v>356</v>
       </c>
-      <c r="AD4" s="554"/>
-      <c r="AE4" s="554"/>
-      <c r="AF4" s="554"/>
+      <c r="AD4" s="553"/>
+      <c r="AE4" s="553"/>
+      <c r="AF4" s="553"/>
       <c r="AG4" s="555"/>
-      <c r="AH4" s="554" t="s">
+      <c r="AH4" s="553" t="s">
         <v>357</v>
       </c>
-      <c r="AI4" s="554"/>
-      <c r="AJ4" s="554"/>
-      <c r="AK4" s="554"/>
+      <c r="AI4" s="553"/>
+      <c r="AJ4" s="553"/>
+      <c r="AK4" s="553"/>
       <c r="AL4" s="555"/>
-      <c r="AM4" s="554" t="s">
+      <c r="AM4" s="553" t="s">
         <v>358</v>
       </c>
-      <c r="AN4" s="554"/>
-      <c r="AO4" s="554"/>
-      <c r="AP4" s="554"/>
+      <c r="AN4" s="553"/>
+      <c r="AO4" s="553"/>
+      <c r="AP4" s="553"/>
       <c r="AQ4" s="555"/>
-      <c r="AR4" s="554" t="s">
+      <c r="AR4" s="553" t="s">
         <v>359</v>
       </c>
-      <c r="AS4" s="554"/>
-      <c r="AT4" s="554"/>
-      <c r="AU4" s="554"/>
+      <c r="AS4" s="553"/>
+      <c r="AT4" s="553"/>
+      <c r="AU4" s="553"/>
       <c r="AV4" s="555"/>
-      <c r="AW4" s="554" t="s">
+      <c r="AW4" s="553" t="s">
         <v>360</v>
       </c>
-      <c r="AX4" s="554"/>
-      <c r="AY4" s="554"/>
-      <c r="AZ4" s="554"/>
-      <c r="BA4" s="554"/>
-      <c r="BB4" s="553" t="s">
+      <c r="AX4" s="553"/>
+      <c r="AY4" s="553"/>
+      <c r="AZ4" s="553"/>
+      <c r="BA4" s="553"/>
+      <c r="BB4" s="554" t="s">
         <v>361</v>
       </c>
-      <c r="BC4" s="554"/>
-      <c r="BD4" s="554"/>
-      <c r="BE4" s="554"/>
+      <c r="BC4" s="553"/>
+      <c r="BD4" s="553"/>
+      <c r="BE4" s="553"/>
       <c r="BF4" s="555"/>
-      <c r="BG4" s="554" t="s">
+      <c r="BG4" s="553" t="s">
         <v>362</v>
       </c>
-      <c r="BH4" s="554"/>
-      <c r="BI4" s="554"/>
-      <c r="BJ4" s="554"/>
-      <c r="BK4" s="554"/>
-      <c r="BL4" s="553" t="s">
+      <c r="BH4" s="553"/>
+      <c r="BI4" s="553"/>
+      <c r="BJ4" s="553"/>
+      <c r="BK4" s="553"/>
+      <c r="BL4" s="554" t="s">
         <v>363</v>
       </c>
-      <c r="BM4" s="554"/>
-      <c r="BN4" s="554"/>
-      <c r="BO4" s="554"/>
-      <c r="BP4" s="554"/>
-      <c r="BQ4" s="553" t="s">
+      <c r="BM4" s="553"/>
+      <c r="BN4" s="553"/>
+      <c r="BO4" s="553"/>
+      <c r="BP4" s="553"/>
+      <c r="BQ4" s="554" t="s">
         <v>364</v>
       </c>
-      <c r="BR4" s="554"/>
-      <c r="BS4" s="554"/>
-      <c r="BT4" s="554"/>
+      <c r="BR4" s="553"/>
+      <c r="BS4" s="553"/>
+      <c r="BT4" s="553"/>
       <c r="BU4" s="555"/>
       <c r="BV4" s="296" t="s">
         <v>365</v>
@@ -47959,6 +47959,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -47971,11 +47976,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -47997,23 +47997,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="560" t="s">
+      <c r="A1" s="562" t="s">
         <v>638</v>
       </c>
-      <c r="B1" s="562" t="s">
+      <c r="B1" s="564" t="s">
         <v>639</v>
       </c>
-      <c r="C1" s="563"/>
-      <c r="D1" s="563"/>
-      <c r="E1" s="563"/>
-      <c r="F1" s="564"/>
-      <c r="G1" s="562" t="s">
+      <c r="C1" s="565"/>
+      <c r="D1" s="565"/>
+      <c r="E1" s="565"/>
+      <c r="F1" s="566"/>
+      <c r="G1" s="564" t="s">
         <v>640</v>
       </c>
-      <c r="H1" s="563"/>
-      <c r="I1" s="563"/>
-      <c r="J1" s="563"/>
-      <c r="K1" s="564"/>
+      <c r="H1" s="565"/>
+      <c r="I1" s="565"/>
+      <c r="J1" s="565"/>
+      <c r="K1" s="566"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -48023,7 +48023,7 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="561"/>
+      <c r="A2" s="563"/>
       <c r="B2" s="466" t="s">
         <v>284</v>
       </c>
@@ -49516,11 +49516,11 @@
       <c r="Y48" t="s">
         <v>689</v>
       </c>
-      <c r="Z48" s="565" t="s">
+      <c r="Z48" s="560" t="s">
         <v>627</v>
       </c>
-      <c r="AA48" s="566"/>
-      <c r="AB48" s="566"/>
+      <c r="AA48" s="561"/>
+      <c r="AB48" s="561"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -49737,11 +49737,11 @@
       <c r="Y53" t="s">
         <v>691</v>
       </c>
-      <c r="Z53" s="565" t="s">
+      <c r="Z53" s="560" t="s">
         <v>626</v>
       </c>
-      <c r="AA53" s="566"/>
-      <c r="AB53" s="566"/>
+      <c r="AA53" s="561"/>
+      <c r="AB53" s="561"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -49943,11 +49943,11 @@
       <c r="Y59" t="s">
         <v>692</v>
       </c>
-      <c r="Z59" s="565" t="s">
+      <c r="Z59" s="560" t="s">
         <v>693</v>
       </c>
-      <c r="AA59" s="566"/>
-      <c r="AB59" s="566"/>
+      <c r="AA59" s="561"/>
+      <c r="AB59" s="561"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="486" t="str">
@@ -50784,17 +50784,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="59" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>